<commit_message>
working on analysis for outline
</commit_message>
<xml_diff>
--- a/data/biomass.xlsx
+++ b/data/biomass.xlsx
@@ -1,30 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE3836A-52CC-3D4D-9DB1-B3D624F056FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="201">
   <si>
     <t>individual</t>
   </si>
@@ -631,6 +624,9 @@
   </si>
   <si>
     <t>CORRAC_166</t>
+  </si>
+  <si>
+    <t>F-C</t>
   </si>
   <si>
     <t>total shoots</t>
@@ -639,8 +635,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -683,6 +679,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -716,11 +718,12 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -737,9 +740,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1066,22 +1066,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E193"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E129" sqref="E129"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.625" style="1"/>
+    <col min="1" max="4" width="10.625" style="1"/>
+    <col min="5" max="5" width="10.625" style="6"/>
+    <col min="6" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1094,119 +1096,122 @@
       <c r="D1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>0.1578</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="6">
         <f>B2+D2</f>
         <v>0.1578</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <f t="shared" ref="E3:E66" si="0">B3+D3</f>
         <v>8.4099999999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>0.11369</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <f t="shared" si="0"/>
         <v>0.11369</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>0.63300000000000001</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <f t="shared" si="0"/>
         <v>0.63300000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>0.18001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>0.18001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>0.14280000000000001</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>0.14280000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>0.19905</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>0.19905</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>0.25972000000000001</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>0.25972000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1214,60 +1219,60 @@
         <f>0.0504+0.0322</f>
         <v>8.2600000000000007E-2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>8.2600000000000007E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>0.12055</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>0.12055</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>0.1202</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>0.1202</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>0.11559999999999999</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>0.11559999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>0.1236</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <f t="shared" si="0"/>
         <v>0.1236</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1275,7 +1280,7 @@
         <f>0.05+0.0395</f>
         <v>8.9499999999999996E-2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="6">
         <f t="shared" si="0"/>
         <v>8.9499999999999996E-2</v>
       </c>
@@ -1287,7 +1292,7 @@
       <c r="B17" s="1">
         <v>9.5680000000000001E-2</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="6">
         <f t="shared" si="0"/>
         <v>9.5680000000000001E-2</v>
       </c>
@@ -1299,7 +1304,7 @@
       <c r="B18" s="1">
         <v>8.4400000000000003E-2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="6">
         <f t="shared" si="0"/>
         <v>8.4400000000000003E-2</v>
       </c>
@@ -1312,7 +1317,7 @@
         <f>0.05+0.021</f>
         <v>7.1000000000000008E-2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="6">
         <f t="shared" si="0"/>
         <v>7.1000000000000008E-2</v>
       </c>
@@ -1324,7 +1329,7 @@
       <c r="B20" s="1">
         <v>5.5550000000000002E-2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="6">
         <f t="shared" si="0"/>
         <v>5.5550000000000002E-2</v>
       </c>
@@ -1336,7 +1341,7 @@
       <c r="B21" s="1">
         <v>9.0660000000000004E-2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="6">
         <f t="shared" si="0"/>
         <v>9.0660000000000004E-2</v>
       </c>
@@ -1348,7 +1353,7 @@
       <c r="B22" s="1">
         <v>0.21970000000000001</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="6">
         <f t="shared" si="0"/>
         <v>0.21970000000000001</v>
       </c>
@@ -1360,7 +1365,7 @@
       <c r="B23" s="1">
         <v>9.826E-2</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>9.826E-2</v>
       </c>
@@ -1372,7 +1377,7 @@
       <c r="B24" s="1">
         <v>6.2850000000000003E-2</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="6">
         <f t="shared" si="0"/>
         <v>6.2850000000000003E-2</v>
       </c>
@@ -1384,7 +1389,7 @@
       <c r="B25" s="1">
         <v>0.10732</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="6">
         <f t="shared" si="0"/>
         <v>0.10732</v>
       </c>
@@ -1396,7 +1401,7 @@
       <c r="B26" s="1">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="6">
         <f t="shared" si="0"/>
         <v>8.5599999999999996E-2</v>
       </c>
@@ -1408,7 +1413,7 @@
       <c r="B27" s="1">
         <v>8.0930000000000002E-2</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="6">
         <f t="shared" si="0"/>
         <v>8.0930000000000002E-2</v>
       </c>
@@ -1420,7 +1425,7 @@
       <c r="B28" s="1">
         <v>0.15595999999999999</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="6">
         <f t="shared" si="0"/>
         <v>0.15595999999999999</v>
       </c>
@@ -1432,7 +1437,7 @@
       <c r="B29" s="1">
         <v>0.92800000000000005</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="6">
         <f t="shared" si="0"/>
         <v>0.92800000000000005</v>
       </c>
@@ -1444,7 +1449,7 @@
       <c r="B30" s="1">
         <v>0.1057</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="6">
         <f t="shared" si="0"/>
         <v>0.1057</v>
       </c>
@@ -1456,7 +1461,7 @@
       <c r="B31" s="1">
         <v>0.11948</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="6">
         <f t="shared" si="0"/>
         <v>0.11948</v>
       </c>
@@ -1468,7 +1473,7 @@
       <c r="B32" s="1">
         <v>0.13216</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="6">
         <f t="shared" si="0"/>
         <v>0.13216</v>
       </c>
@@ -1480,7 +1485,7 @@
       <c r="B33" s="1">
         <v>0.1056</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="6">
         <f t="shared" si="0"/>
         <v>0.1056</v>
       </c>
@@ -1492,7 +1497,7 @@
       <c r="B34" s="1">
         <v>0.6976</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="6">
         <f t="shared" si="0"/>
         <v>0.6976</v>
       </c>
@@ -1504,7 +1509,7 @@
       <c r="B35" s="1">
         <v>0.33112000000000003</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="6">
         <f t="shared" si="0"/>
         <v>0.33112000000000003</v>
       </c>
@@ -1516,7 +1521,7 @@
       <c r="B36" s="1">
         <v>0.39595000000000002</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="6">
         <f t="shared" si="0"/>
         <v>0.39595000000000002</v>
       </c>
@@ -1528,7 +1533,7 @@
       <c r="B37" s="1">
         <v>0.45728999999999997</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="6">
         <f t="shared" si="0"/>
         <v>0.45728999999999997</v>
       </c>
@@ -1540,7 +1545,7 @@
       <c r="B38" s="1">
         <v>0.22020000000000001</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="6">
         <f t="shared" si="0"/>
         <v>0.22020000000000001</v>
       </c>
@@ -1552,7 +1557,7 @@
       <c r="B39" s="1">
         <v>0.28299999999999997</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="6">
         <f t="shared" si="0"/>
         <v>0.28299999999999997</v>
       </c>
@@ -1564,7 +1569,7 @@
       <c r="B40" s="1">
         <v>0.37919999999999998</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="6">
         <f t="shared" si="0"/>
         <v>0.37919999999999998</v>
       </c>
@@ -1576,7 +1581,7 @@
       <c r="B41" s="1">
         <v>0.21654000000000001</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="6">
         <f t="shared" si="0"/>
         <v>0.21654000000000001</v>
       </c>
@@ -1588,7 +1593,7 @@
       <c r="B42" s="1">
         <v>0.15306</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="6">
         <f t="shared" si="0"/>
         <v>0.15306</v>
       </c>
@@ -1600,7 +1605,7 @@
       <c r="B43" s="1">
         <v>0.11425</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="6">
         <f t="shared" si="0"/>
         <v>0.11425</v>
       </c>
@@ -1612,7 +1617,7 @@
       <c r="B44" s="1">
         <v>0.1731</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="6">
         <f t="shared" si="0"/>
         <v>0.1731</v>
       </c>
@@ -1624,7 +1629,7 @@
       <c r="B45" s="1">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="6">
         <f t="shared" si="0"/>
         <v>0.13700000000000001</v>
       </c>
@@ -1636,7 +1641,7 @@
       <c r="B46" s="1">
         <v>6.0600000000000001E-2</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="6">
         <f t="shared" si="0"/>
         <v>6.0600000000000001E-2</v>
       </c>
@@ -1648,7 +1653,7 @@
       <c r="B47" s="1">
         <v>0.1275</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="6">
         <f t="shared" si="0"/>
         <v>0.1275</v>
       </c>
@@ -1660,7 +1665,7 @@
       <c r="B48" s="1">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="6">
         <f t="shared" si="0"/>
         <v>5.5500000000000001E-2</v>
       </c>
@@ -1672,7 +1677,7 @@
       <c r="B49" s="1">
         <v>0.18284</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="6">
         <f t="shared" si="0"/>
         <v>0.18284</v>
       </c>
@@ -1684,7 +1689,7 @@
       <c r="B50" s="1">
         <v>0.17377999999999999</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="6">
         <f t="shared" si="0"/>
         <v>0.17377999999999999</v>
       </c>
@@ -1696,7 +1701,7 @@
       <c r="B51" s="1">
         <v>8.9099999999999999E-2</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="6">
         <f t="shared" si="0"/>
         <v>8.9099999999999999E-2</v>
       </c>
@@ -1708,7 +1713,7 @@
       <c r="B52" s="1">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="6">
         <f t="shared" si="0"/>
         <v>8.4099999999999994E-2</v>
       </c>
@@ -1720,7 +1725,7 @@
       <c r="B53" s="1">
         <v>6.9699999999999998E-2</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="6">
         <f t="shared" si="0"/>
         <v>6.9699999999999998E-2</v>
       </c>
@@ -1735,7 +1740,7 @@
       <c r="C54" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="6">
         <f t="shared" si="0"/>
         <v>3.7199999999999997E-2</v>
       </c>
@@ -1750,7 +1755,7 @@
       <c r="C55" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="6">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
@@ -1763,7 +1768,7 @@
         <v>0.47</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="E56" s="1">
+      <c r="E56" s="6">
         <f t="shared" si="0"/>
         <v>0.47</v>
       </c>
@@ -1775,7 +1780,7 @@
       <c r="B57" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E57" s="1" t="e">
+      <c r="E57" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -1790,7 +1795,7 @@
       <c r="C58" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="6">
         <f t="shared" si="0"/>
         <v>0.44400000000000001</v>
       </c>
@@ -1802,7 +1807,7 @@
       <c r="B59" s="1">
         <v>0.4834</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="6">
         <f t="shared" si="0"/>
         <v>0.4834</v>
       </c>
@@ -1817,7 +1822,7 @@
       <c r="C60" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="6">
         <f t="shared" si="0"/>
         <v>3.3399999999999999E-2</v>
       </c>
@@ -1829,7 +1834,7 @@
       <c r="B61" s="1">
         <v>9.5170000000000005E-2</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="6">
         <f t="shared" si="0"/>
         <v>9.5170000000000005E-2</v>
       </c>
@@ -1841,7 +1846,7 @@
       <c r="B62" s="1">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="6">
         <f t="shared" si="0"/>
         <v>7.3599999999999999E-2</v>
       </c>
@@ -1856,7 +1861,7 @@
       <c r="C63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="6">
         <f t="shared" si="0"/>
         <v>4.02E-2</v>
       </c>
@@ -1868,7 +1873,7 @@
       <c r="B64" s="1">
         <v>6.0100000000000001E-2</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="6">
         <f t="shared" si="0"/>
         <v>6.0100000000000001E-2</v>
       </c>
@@ -1883,7 +1888,7 @@
       <c r="C65" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="6">
         <f t="shared" si="0"/>
         <v>2.6499999999999999E-2</v>
       </c>
@@ -1895,7 +1900,7 @@
       <c r="B66" s="1">
         <v>0.12623000000000001</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="6">
         <f t="shared" si="0"/>
         <v>0.12623000000000001</v>
       </c>
@@ -1907,7 +1912,7 @@
       <c r="B67" s="1">
         <v>0.19574</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="6">
         <f t="shared" ref="E67:E130" si="1">B67+D67</f>
         <v>0.19574</v>
       </c>
@@ -1919,7 +1924,7 @@
       <c r="B68" s="1">
         <v>0.16908000000000001</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="6">
         <f t="shared" si="1"/>
         <v>0.16908000000000001</v>
       </c>
@@ -1931,7 +1936,7 @@
       <c r="B69" s="1">
         <v>5.7930000000000002E-2</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="6">
         <f t="shared" si="1"/>
         <v>5.7930000000000002E-2</v>
       </c>
@@ -1943,7 +1948,7 @@
       <c r="B70" s="1">
         <v>0.14298</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="6">
         <f t="shared" si="1"/>
         <v>0.14298</v>
       </c>
@@ -1955,7 +1960,7 @@
       <c r="B71" s="1">
         <v>9.5149999999999998E-2</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="6">
         <f t="shared" si="1"/>
         <v>9.5149999999999998E-2</v>
       </c>
@@ -1967,7 +1972,7 @@
       <c r="B72" s="1">
         <v>0.1221</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="6">
         <f t="shared" si="1"/>
         <v>0.1221</v>
       </c>
@@ -1979,7 +1984,7 @@
       <c r="B73" s="1">
         <v>0.10866000000000001</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="6">
         <f t="shared" si="1"/>
         <v>0.10866000000000001</v>
       </c>
@@ -1991,7 +1996,7 @@
       <c r="B74" s="1">
         <v>0.11178</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="6">
         <f t="shared" si="1"/>
         <v>0.11178</v>
       </c>
@@ -2003,7 +2008,7 @@
       <c r="B75" s="1">
         <v>0.11191</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="6">
         <f t="shared" si="1"/>
         <v>0.11191</v>
       </c>
@@ -2015,7 +2020,7 @@
       <c r="B76" s="1">
         <v>0.12363</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="6">
         <f t="shared" si="1"/>
         <v>0.12363</v>
       </c>
@@ -2027,7 +2032,7 @@
       <c r="B77" s="1">
         <v>8.3280000000000007E-2</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="6">
         <f t="shared" si="1"/>
         <v>8.3280000000000007E-2</v>
       </c>
@@ -2039,7 +2044,7 @@
       <c r="B78" s="1">
         <v>0.12200999999999999</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="6">
         <f t="shared" si="1"/>
         <v>0.12200999999999999</v>
       </c>
@@ -2051,7 +2056,7 @@
       <c r="B79" s="1">
         <v>0.19725000000000001</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="6">
         <f t="shared" si="1"/>
         <v>0.19725000000000001</v>
       </c>
@@ -2063,7 +2068,7 @@
       <c r="B80" s="1">
         <v>0.11362</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="6">
         <f t="shared" si="1"/>
         <v>0.11362</v>
       </c>
@@ -2075,7 +2080,7 @@
       <c r="B81" s="1">
         <v>9.8710000000000006E-2</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="6">
         <f t="shared" si="1"/>
         <v>9.8710000000000006E-2</v>
       </c>
@@ -2087,7 +2092,7 @@
       <c r="B82" s="1">
         <v>0.71364000000000005</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="6">
         <f t="shared" si="1"/>
         <v>0.71364000000000005</v>
       </c>
@@ -2099,7 +2104,7 @@
       <c r="B83" s="1">
         <v>0.46990999999999999</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="6">
         <f t="shared" si="1"/>
         <v>0.46990999999999999</v>
       </c>
@@ -2111,7 +2116,7 @@
       <c r="B84" s="1">
         <v>0.41602</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="6">
         <f t="shared" si="1"/>
         <v>0.41602</v>
       </c>
@@ -2123,7 +2128,7 @@
       <c r="B85" s="1">
         <v>0.49452000000000002</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="6">
         <f t="shared" si="1"/>
         <v>0.49452000000000002</v>
       </c>
@@ -2135,7 +2140,7 @@
       <c r="B86" s="1">
         <v>0.58830000000000005</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="6">
         <f t="shared" si="1"/>
         <v>0.58830000000000005</v>
       </c>
@@ -2147,7 +2152,7 @@
       <c r="B87" s="1">
         <v>0.44529999999999997</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="6">
         <f t="shared" si="1"/>
         <v>0.44529999999999997</v>
       </c>
@@ -2159,7 +2164,7 @@
       <c r="B88" s="1">
         <v>0.16341</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88" s="6">
         <f t="shared" si="1"/>
         <v>0.16341</v>
       </c>
@@ -2171,7 +2176,7 @@
       <c r="B89" s="1">
         <v>0.30271999999999999</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89" s="6">
         <f t="shared" si="1"/>
         <v>0.30271999999999999</v>
       </c>
@@ -2183,7 +2188,7 @@
       <c r="B90" s="1">
         <v>0.39</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90" s="6">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
@@ -2195,7 +2200,7 @@
       <c r="B91" s="1">
         <v>0.2732</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91" s="6">
         <f t="shared" si="1"/>
         <v>0.2732</v>
       </c>
@@ -2207,7 +2212,7 @@
       <c r="B92" s="1">
         <v>0.18314</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92" s="6">
         <f t="shared" si="1"/>
         <v>0.18314</v>
       </c>
@@ -2219,7 +2224,7 @@
       <c r="B93" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E93" s="1" t="e">
+      <c r="E93" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2231,7 +2236,7 @@
       <c r="B94" s="1">
         <v>0.49746000000000001</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94" s="6">
         <f t="shared" si="1"/>
         <v>0.49746000000000001</v>
       </c>
@@ -2243,7 +2248,7 @@
       <c r="B95" s="1">
         <v>0.36220000000000002</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95" s="6">
         <f t="shared" si="1"/>
         <v>0.36220000000000002</v>
       </c>
@@ -2255,7 +2260,7 @@
       <c r="B96" s="1">
         <v>0.51102999999999998</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="6">
         <f t="shared" si="1"/>
         <v>0.51102999999999998</v>
       </c>
@@ -2267,7 +2272,7 @@
       <c r="B97" s="1">
         <v>0.47699999999999998</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97" s="6">
         <f t="shared" si="1"/>
         <v>0.47699999999999998</v>
       </c>
@@ -2279,7 +2284,7 @@
       <c r="B98" s="1">
         <v>0.11364</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98" s="6">
         <f t="shared" si="1"/>
         <v>0.11364</v>
       </c>
@@ -2291,7 +2296,7 @@
       <c r="B99" s="1">
         <v>0.14896999999999999</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99" s="6">
         <f t="shared" si="1"/>
         <v>0.14896999999999999</v>
       </c>
@@ -2303,7 +2308,7 @@
       <c r="B100" s="1">
         <v>8.6440000000000003E-2</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100" s="6">
         <f t="shared" si="1"/>
         <v>8.6440000000000003E-2</v>
       </c>
@@ -2315,7 +2320,7 @@
       <c r="B101" s="1">
         <v>0.14696000000000001</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="6">
         <f t="shared" si="1"/>
         <v>0.14696000000000001</v>
       </c>
@@ -2327,7 +2332,7 @@
       <c r="B102" s="1">
         <v>0.11192000000000001</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="6">
         <f t="shared" si="1"/>
         <v>0.11192000000000001</v>
       </c>
@@ -2339,7 +2344,7 @@
       <c r="B103" s="1">
         <v>0.11283</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103" s="6">
         <f t="shared" si="1"/>
         <v>0.11283</v>
       </c>
@@ -2351,7 +2356,7 @@
       <c r="B104" s="1">
         <v>0.114523</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="6">
         <f t="shared" si="1"/>
         <v>0.114523</v>
       </c>
@@ -2363,7 +2368,7 @@
       <c r="B105" s="1">
         <v>0.10299999999999999</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="6">
         <f t="shared" si="1"/>
         <v>0.10299999999999999</v>
       </c>
@@ -2375,7 +2380,7 @@
       <c r="B106" s="1">
         <v>0.10724</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="6">
         <f t="shared" si="1"/>
         <v>0.10724</v>
       </c>
@@ -2387,7 +2392,7 @@
       <c r="B107" s="1">
         <v>9.7339999999999996E-2</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="6">
         <f t="shared" si="1"/>
         <v>9.7339999999999996E-2</v>
       </c>
@@ -2399,7 +2404,7 @@
       <c r="B108" s="1">
         <v>0.11348</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="6">
         <f t="shared" si="1"/>
         <v>0.11348</v>
       </c>
@@ -2411,7 +2416,7 @@
       <c r="B109" s="1">
         <v>7.4529999999999999E-2</v>
       </c>
-      <c r="E109" s="1">
+      <c r="E109" s="6">
         <f t="shared" si="1"/>
         <v>7.4529999999999999E-2</v>
       </c>
@@ -2423,7 +2428,7 @@
       <c r="B110" s="1">
         <v>0.11441</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="6">
         <f t="shared" si="1"/>
         <v>0.11441</v>
       </c>
@@ -2435,7 +2440,7 @@
       <c r="B111" s="1">
         <v>0.10153</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111" s="6">
         <f t="shared" si="1"/>
         <v>0.10153</v>
       </c>
@@ -2447,7 +2452,7 @@
       <c r="B112" s="1">
         <v>9.1689999999999994E-2</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112" s="6">
         <f t="shared" si="1"/>
         <v>9.1689999999999994E-2</v>
       </c>
@@ -2459,7 +2464,7 @@
       <c r="B113" s="1">
         <v>0.1221</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113" s="6">
         <f t="shared" si="1"/>
         <v>0.1221</v>
       </c>
@@ -2471,7 +2476,7 @@
       <c r="B114" s="1">
         <v>3.8440000000000002E-2</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="6">
         <f t="shared" si="1"/>
         <v>3.8440000000000002E-2</v>
       </c>
@@ -2483,7 +2488,7 @@
       <c r="B115" s="1">
         <v>5.3719999999999997E-2</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115" s="6">
         <f t="shared" si="1"/>
         <v>5.3719999999999997E-2</v>
       </c>
@@ -2495,7 +2500,7 @@
       <c r="B116" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E116" s="1" t="e">
+      <c r="E116" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2507,7 +2512,7 @@
       <c r="B117" s="1">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117" s="6">
         <f t="shared" si="1"/>
         <v>4.9099999999999998E-2</v>
       </c>
@@ -2519,7 +2524,7 @@
       <c r="B118" s="1">
         <v>4.1309999999999999E-2</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118" s="6">
         <f t="shared" si="1"/>
         <v>4.1309999999999999E-2</v>
       </c>
@@ -2531,7 +2536,7 @@
       <c r="B119" s="1">
         <v>2.5819999999999999E-2</v>
       </c>
-      <c r="E119" s="1">
+      <c r="E119" s="6">
         <f t="shared" si="1"/>
         <v>2.5819999999999999E-2</v>
       </c>
@@ -2549,7 +2554,7 @@
       <c r="D120" s="1">
         <v>5.9350699999999996</v>
       </c>
-      <c r="E120" s="1">
+      <c r="E120" s="6">
         <f t="shared" si="1"/>
         <v>6.0126099999999996</v>
       </c>
@@ -2561,7 +2566,7 @@
       <c r="B121" s="1">
         <v>2.2429999999999999E-2</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E121" s="6">
         <f t="shared" si="1"/>
         <v>2.2429999999999999E-2</v>
       </c>
@@ -2573,7 +2578,7 @@
       <c r="B122" s="1">
         <v>4.1459999999999997E-2</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="6">
         <f t="shared" si="1"/>
         <v>4.1459999999999997E-2</v>
       </c>
@@ -2585,7 +2590,7 @@
       <c r="B123" s="1">
         <v>8.9440000000000006E-2</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="6">
         <f t="shared" si="1"/>
         <v>8.9440000000000006E-2</v>
       </c>
@@ -2597,7 +2602,7 @@
       <c r="B124" s="1">
         <v>4.2770000000000002E-2</v>
       </c>
-      <c r="E124" s="1">
+      <c r="E124" s="6">
         <f t="shared" si="1"/>
         <v>4.2770000000000002E-2</v>
       </c>
@@ -2609,7 +2614,7 @@
       <c r="B125" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E125" s="1" t="e">
+      <c r="E125" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2621,7 +2626,7 @@
       <c r="B126" s="1">
         <v>6.2140000000000001E-2</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="6">
         <f t="shared" si="1"/>
         <v>6.2140000000000001E-2</v>
       </c>
@@ -2633,7 +2638,7 @@
       <c r="B127" s="1">
         <v>6.8339999999999998E-2</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127" s="6">
         <f t="shared" si="1"/>
         <v>6.8339999999999998E-2</v>
       </c>
@@ -2645,12 +2650,12 @@
       <c r="B128" s="1">
         <v>6.3759999999999997E-2</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128" s="6">
         <f t="shared" si="1"/>
         <v>6.3759999999999997E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>132</v>
       </c>
@@ -2663,487 +2668,622 @@
       <c r="D129" s="1">
         <v>6.0713499999999998</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129" s="6">
         <f t="shared" si="1"/>
         <v>6.1383200000000002</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B130" s="1">
         <v>0.19220999999999999</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130" s="6">
         <f t="shared" si="1"/>
         <v>0.19220999999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130" s="1">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B131" s="1">
         <v>0.16100999999999999</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131" s="6">
         <f t="shared" ref="E131:E193" si="2">B131+D131</f>
         <v>0.16100999999999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131" s="1">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B132" s="1">
         <v>0.10818</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132" s="6">
         <f t="shared" si="2"/>
         <v>0.10818</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132" s="1">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="1">
         <v>0.14993999999999999</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133" s="6">
         <f t="shared" si="2"/>
         <v>0.14993999999999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133" s="1">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B134" s="1">
         <v>0.12035999999999999</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134" s="6">
         <f t="shared" si="2"/>
         <v>0.12035999999999999</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134" s="1">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B135" s="1">
         <v>0.12628</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135" s="6">
         <f t="shared" si="2"/>
         <v>0.12628</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135" s="1">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B136" s="1">
         <v>9.0279999999999999E-2</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136" s="6">
         <f t="shared" si="2"/>
         <v>9.0279999999999999E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B137" s="1">
         <v>0.16172</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="6">
         <f t="shared" si="2"/>
         <v>0.16172</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B138" s="1">
         <v>0.29918</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138" s="6">
         <f t="shared" si="2"/>
         <v>0.29918</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B139" s="1">
         <v>0.18142</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139" s="6">
         <f t="shared" si="2"/>
         <v>0.18142</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139" s="1">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B140" s="1">
         <v>0.40621000000000002</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140" s="6">
         <f t="shared" si="2"/>
         <v>0.40621000000000002</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B141" s="1">
         <v>0.29359000000000002</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141" s="6">
         <f t="shared" si="2"/>
         <v>0.29359000000000002</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141" s="1">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B142" s="1">
         <v>0.20619000000000001</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142" s="6">
         <f t="shared" si="2"/>
         <v>0.20619000000000001</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B143" s="1">
         <v>0.16874</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143" s="6">
         <f t="shared" si="2"/>
         <v>0.16874</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>147</v>
       </c>
       <c r="B144" s="1">
         <v>0.15673999999999999</v>
       </c>
-      <c r="E144" s="1">
+      <c r="E144" s="6">
         <f t="shared" si="2"/>
         <v>0.15673999999999999</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B145" s="1">
         <v>0.20263</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145" s="6">
         <f t="shared" si="2"/>
         <v>0.20263</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145" s="1">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>149</v>
       </c>
       <c r="B146" s="1">
         <v>0.27638000000000001</v>
       </c>
-      <c r="E146" s="1">
+      <c r="E146" s="6">
         <f t="shared" si="2"/>
         <v>0.27638000000000001</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146" s="1">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B147" s="1">
         <v>6.2740000000000004E-2</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147" s="6">
         <f t="shared" si="2"/>
         <v>6.2740000000000004E-2</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B148" s="1">
         <v>0.15723999999999999</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148" s="6">
         <f t="shared" si="2"/>
         <v>0.15723999999999999</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148" s="1">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E149" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="1">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E149" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F149" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E150" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="1">
+        <v>0.14215</v>
+      </c>
+      <c r="E150" s="6">
+        <f t="shared" si="2"/>
+        <v>0.14215</v>
+      </c>
+      <c r="F150" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E151" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B151" s="1">
+        <v>0.19455</v>
+      </c>
+      <c r="E151" s="6">
+        <f t="shared" si="2"/>
+        <v>0.19455</v>
+      </c>
+      <c r="F151" s="1">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E152" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B152" s="1">
+        <v>9.3380000000000005E-2</v>
+      </c>
+      <c r="E152" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3380000000000005E-2</v>
+      </c>
+      <c r="F152" s="1">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E153" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B153" s="1">
+        <v>0.21836</v>
+      </c>
+      <c r="E153" s="6">
+        <f t="shared" si="2"/>
+        <v>0.21836</v>
+      </c>
+      <c r="F153" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E154" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="1">
+        <v>0.24346999999999999</v>
+      </c>
+      <c r="E154" s="6">
+        <f t="shared" si="2"/>
+        <v>0.24346999999999999</v>
+      </c>
+      <c r="F154" s="1">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E155" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B155" s="1">
+        <v>0.20174</v>
+      </c>
+      <c r="E155" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20174</v>
+      </c>
+      <c r="F155" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E156" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B156" s="1">
+        <v>0.1925</v>
+      </c>
+      <c r="E156" s="6">
+        <f t="shared" si="2"/>
+        <v>0.1925</v>
+      </c>
+      <c r="F156" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E157" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B157" s="1">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="E157" s="6">
+        <f t="shared" si="2"/>
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="F157" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E158" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B158" s="1">
+        <v>0.15851999999999999</v>
+      </c>
+      <c r="E158" s="6">
+        <f t="shared" si="2"/>
+        <v>0.15851999999999999</v>
+      </c>
+      <c r="F158" s="1">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E159" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B159" s="1">
+        <v>0.13694000000000001</v>
+      </c>
+      <c r="E159" s="6">
+        <f t="shared" si="2"/>
+        <v>0.13694000000000001</v>
+      </c>
+      <c r="F159" s="1">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E160" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B160" s="1">
+        <v>0.44784000000000002</v>
+      </c>
+      <c r="E160" s="6">
+        <f t="shared" si="2"/>
+        <v>0.44784000000000002</v>
+      </c>
+      <c r="F160" s="1">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E161" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B161" s="1">
+        <v>0.21001</v>
+      </c>
+      <c r="E161" s="6">
+        <f t="shared" si="2"/>
+        <v>0.21001</v>
+      </c>
+      <c r="F161" s="1">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E163" s="1">
+      <c r="E163" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E164" s="1">
+      <c r="E164" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E165" s="1">
+      <c r="E165" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E166" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E167" s="1">
+      <c r="E167" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E168" s="1">
+      <c r="E168" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E169" s="1">
+      <c r="E169" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E170" s="1">
+      <c r="E170" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E171" s="1">
+      <c r="E171" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E172" s="1">
+      <c r="E172" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E173" s="1">
+      <c r="E173" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E174" s="1">
+      <c r="E174" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E175" s="1">
+      <c r="E175" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E176" s="1">
+      <c r="E176" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3158,7 +3298,7 @@
       <c r="D177" s="1">
         <v>8.2289999999999992</v>
       </c>
-      <c r="E177" s="1">
+      <c r="E177" s="6">
         <f t="shared" si="2"/>
         <v>8.2289999999999992</v>
       </c>
@@ -3167,7 +3307,7 @@
       <c r="A178" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E178" s="1">
+      <c r="E178" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3176,7 +3316,7 @@
       <c r="A179" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E179" s="1">
+      <c r="E179" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3185,7 +3325,7 @@
       <c r="A180" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E180" s="1">
+      <c r="E180" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3194,7 +3334,7 @@
       <c r="A181" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E181" s="1">
+      <c r="E181" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3203,7 +3343,7 @@
       <c r="A182" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E182" s="1">
+      <c r="E182" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3212,7 +3352,7 @@
       <c r="A183" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E183" s="1">
+      <c r="E183" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3221,7 +3361,7 @@
       <c r="A184" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E184" s="1">
+      <c r="E184" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3230,7 +3370,7 @@
       <c r="A185" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E185" s="1">
+      <c r="E185" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3239,7 +3379,7 @@
       <c r="A186" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E186" s="1">
+      <c r="E186" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3248,7 +3388,7 @@
       <c r="A187" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E187" s="1">
+      <c r="E187" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3257,7 +3397,7 @@
       <c r="A188" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E188" s="1">
+      <c r="E188" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3270,7 +3410,7 @@
         <f>12.688+11.96</f>
         <v>24.648000000000003</v>
       </c>
-      <c r="E189" s="1">
+      <c r="E189" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3279,7 +3419,7 @@
       <c r="A190" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E190" s="1">
+      <c r="E190" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3288,7 +3428,7 @@
       <c r="A191" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E191" s="1">
+      <c r="E191" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3297,7 +3437,7 @@
       <c r="A192" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E192" s="1">
+      <c r="E192" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3306,7 +3446,7 @@
       <c r="A193" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E193" s="1">
+      <c r="E193" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
more weights and obs
</commit_message>
<xml_diff>
--- a/data/biomass.xlsx
+++ b/data/biomass.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/chillfreeze/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC4431A-621C-2F4C-B95A-6DC2EB304C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="460" windowWidth="22720" windowHeight="13440" tabRatio="500"/>
+    <workbookView xWindow="15020" yWindow="8440" windowWidth="22720" windowHeight="13440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="250">
   <si>
     <t>individual</t>
   </si>
@@ -642,18 +649,163 @@
   </si>
   <si>
     <t>SORAME_146</t>
+  </si>
+  <si>
+    <t>ACEPEN_156</t>
+  </si>
+  <si>
+    <t>ACEPEN_16</t>
+  </si>
+  <si>
+    <t>ACEPEN_26</t>
+  </si>
+  <si>
+    <t>ACEPEN_36</t>
+  </si>
+  <si>
+    <t>ACEPEN_46</t>
+  </si>
+  <si>
+    <t>ACEPEN_56</t>
+  </si>
+  <si>
+    <t>ACEPEN_66</t>
+  </si>
+  <si>
+    <t>ACEPEN_76</t>
+  </si>
+  <si>
+    <t>ACEPEN_86</t>
+  </si>
+  <si>
+    <t>ACEPEN_96</t>
+  </si>
+  <si>
+    <t>ACEPEN_106</t>
+  </si>
+  <si>
+    <t>ACEPEN_116</t>
+  </si>
+  <si>
+    <t>ACEPEN_126</t>
+  </si>
+  <si>
+    <t>ACEPEN_136</t>
+  </si>
+  <si>
+    <t>ACEPEN_146</t>
+  </si>
+  <si>
+    <t>ACEPEN_166</t>
+  </si>
+  <si>
+    <t>CORRAC_18</t>
+  </si>
+  <si>
+    <t>CORRAC_28</t>
+  </si>
+  <si>
+    <t>CORRAC_38</t>
+  </si>
+  <si>
+    <t>CORRAC_48</t>
+  </si>
+  <si>
+    <t>CORRAC_58</t>
+  </si>
+  <si>
+    <t>CORRAC_68</t>
+  </si>
+  <si>
+    <t>CORRAC_78</t>
+  </si>
+  <si>
+    <t>CORRAC_88</t>
+  </si>
+  <si>
+    <t>CORRAC_98</t>
+  </si>
+  <si>
+    <t>CORRAC_108</t>
+  </si>
+  <si>
+    <t>CORRAC_118</t>
+  </si>
+  <si>
+    <t>CORRAC_128</t>
+  </si>
+  <si>
+    <t>CORRAC_138</t>
+  </si>
+  <si>
+    <t>CORRAC_148</t>
+  </si>
+  <si>
+    <t>CORRAC_158</t>
+  </si>
+  <si>
+    <t>CORRAC_168</t>
+  </si>
+  <si>
+    <t>SORAME_26</t>
+  </si>
+  <si>
+    <t>SORAME_36</t>
+  </si>
+  <si>
+    <t>SORAME_46</t>
+  </si>
+  <si>
+    <t>SORAME_56</t>
+  </si>
+  <si>
+    <t>SORAME_66</t>
+  </si>
+  <si>
+    <t>SORAME_76</t>
+  </si>
+  <si>
+    <t>SORAME_86</t>
+  </si>
+  <si>
+    <t>SORAME_96</t>
+  </si>
+  <si>
+    <t>SORAME_106</t>
+  </si>
+  <si>
+    <t>SORAME_116</t>
+  </si>
+  <si>
+    <t>SORAME_126</t>
+  </si>
+  <si>
+    <t>SORAME_136</t>
+  </si>
+  <si>
+    <t>SORAME_156</t>
+  </si>
+  <si>
+    <t>SORAME_166</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Black"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -737,11 +889,12 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -760,6 +913,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1086,14 +1242,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" activeCell="D188" sqref="D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1287,7 @@
         <v>0.11425</v>
       </c>
       <c r="E2" s="6">
-        <f t="shared" ref="E2:E35" si="0">B2+D2</f>
+        <f t="shared" ref="E2:E51" si="0">B2+D2</f>
         <v>0.11425</v>
       </c>
     </row>
@@ -1268,9 +1424,15 @@
       <c r="B13" s="1">
         <v>0.22020000000000001</v>
       </c>
+      <c r="C13" s="1">
+        <v>2.6230000000000002</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>0.22020000000000001</v>
+        <v>0.79020000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1322,2218 +1484,2681 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.3720000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.923</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.1919999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B34" s="1">
         <v>0.2732</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E34" s="6">
         <f t="shared" si="0"/>
         <v>0.2732</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B35" s="1">
         <v>0.18314</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E35" s="6">
         <f t="shared" si="0"/>
         <v>0.18314</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="6" t="e">
+      <c r="E36" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B37" s="1">
         <v>0.49746000000000001</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E37" s="6">
         <f t="shared" si="0"/>
         <v>0.49746000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B38" s="1">
         <v>0.71364000000000005</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E38" s="6">
         <f t="shared" si="0"/>
         <v>0.71364000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B39" s="1">
         <v>0.36220000000000002</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E39" s="6">
         <f t="shared" si="0"/>
         <v>0.36220000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B40" s="1">
         <v>0.51102999999999998</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E40" s="6">
         <f t="shared" si="0"/>
         <v>0.51102999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B41" s="1">
         <v>0.47699999999999998</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E41" s="6">
         <f t="shared" si="0"/>
         <v>0.47699999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B42" s="1">
         <v>0.46990999999999999</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E42" s="6">
         <f t="shared" si="0"/>
         <v>0.46990999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B43" s="1">
         <v>0.41602</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E43" s="6">
         <f t="shared" si="0"/>
         <v>0.41602</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B44" s="1">
         <v>0.49452000000000002</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E44" s="6">
         <f t="shared" si="0"/>
         <v>0.49452000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B45" s="1">
         <v>0.58830000000000005</v>
       </c>
-      <c r="E29" s="6">
-        <f t="shared" si="0"/>
-        <v>0.58830000000000005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="E45" s="6">
+        <f>B45+D73</f>
+        <v>3.5942999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B46" s="1">
         <v>0.44529999999999997</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E46" s="6">
         <f t="shared" si="0"/>
         <v>0.44529999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B47" s="1">
         <v>0.16341</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E47" s="6">
         <f t="shared" si="0"/>
         <v>0.16341</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B48" s="1">
         <v>0.30271999999999999</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E48" s="6">
         <f t="shared" si="0"/>
         <v>0.30271999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B49" s="1">
         <v>0.39</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E49" s="6">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B50" s="1">
         <f>0.0504+0.0322</f>
         <v>8.2600000000000007E-2</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E50" s="6">
         <f t="shared" si="0"/>
         <v>8.2600000000000007E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B51" s="1">
         <v>0.18142</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C51" s="1">
         <v>7.62</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D51" s="1">
         <v>4.6589999999999998</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E51" s="6">
         <f t="shared" si="0"/>
         <v>4.8404199999999999</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F51" s="1">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C52" s="1">
         <v>11.35</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D52" s="1">
         <v>5.6225500000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B53" s="1">
         <v>0.12055</v>
       </c>
-      <c r="E37" s="6">
-        <f t="shared" ref="E37:E58" si="1">B37+D37</f>
+      <c r="E53" s="6">
+        <f t="shared" ref="E53:E74" si="1">B53+D53</f>
         <v>0.12055</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B54" s="1">
         <v>0.40621000000000002</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E54" s="6">
         <f t="shared" si="1"/>
         <v>0.40621000000000002</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F54" s="1">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B55" s="1">
         <v>0.1202</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E55" s="6">
         <f t="shared" si="1"/>
         <v>0.1202</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B56" s="1">
         <v>0.29359000000000002</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E56" s="6">
         <f t="shared" si="1"/>
         <v>0.29359000000000002</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F56" s="1">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B57" s="1">
         <v>0.11559999999999999</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E57" s="6">
         <f t="shared" si="1"/>
         <v>0.11559999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B58" s="1">
         <v>0.20619000000000001</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E58" s="6">
         <f t="shared" si="1"/>
         <v>0.20619000000000001</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F58" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B59" s="1">
         <v>0.1578</v>
       </c>
-      <c r="E43" s="6">
+      <c r="C59" s="1">
+        <v>13.93</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2.7090000000000001</v>
+      </c>
+      <c r="E59" s="6">
         <f t="shared" si="1"/>
-        <v>0.1578</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+        <v>2.8668</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B60" s="1">
         <v>0.1236</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E60" s="6">
         <f t="shared" si="1"/>
         <v>0.1236</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B61" s="1">
         <v>0.16874</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E61" s="6">
         <f t="shared" si="1"/>
         <v>0.16874</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F61" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B62" s="1">
         <f>0.05+0.0395</f>
         <v>8.9499999999999996E-2</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E62" s="6">
         <f t="shared" si="1"/>
         <v>8.9499999999999996E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B63" s="1">
         <v>0.15673999999999999</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E63" s="6">
         <f t="shared" si="1"/>
         <v>0.15673999999999999</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F63" s="1">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B64" s="1">
         <v>0.19220999999999999</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E64" s="6">
         <f t="shared" si="1"/>
         <v>0.19220999999999999</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F64" s="1">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B65" s="1">
         <v>9.5680000000000001E-2</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E65" s="6">
         <f t="shared" si="1"/>
         <v>9.5680000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B66" s="1">
         <v>0.20263</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E66" s="6">
         <f t="shared" si="1"/>
         <v>0.20263</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F66" s="1">
         <v>-0.11</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B67" s="1">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E67" s="6">
         <f t="shared" si="1"/>
         <v>8.4099999999999994E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B68" s="1">
         <v>0.16100999999999999</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E68" s="6">
         <f t="shared" si="1"/>
         <v>0.16100999999999999</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F68" s="1">
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B69" s="1">
         <v>0.11369</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E69" s="6">
         <f t="shared" si="1"/>
         <v>0.11369</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B70" s="1">
         <v>0.10818</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E70" s="6">
         <f t="shared" si="1"/>
         <v>0.10818</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F70" s="1">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B71" s="1">
         <v>0.63300000000000001</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E71" s="6">
         <f t="shared" si="1"/>
         <v>0.63300000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B72" s="1">
         <v>0.14993999999999999</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E72" s="6">
         <f t="shared" si="1"/>
         <v>0.14993999999999999</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F72" s="1">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B73" s="1">
         <v>0.18001</v>
       </c>
-      <c r="E57" s="6">
-        <f t="shared" si="1"/>
-        <v>0.18001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="C73" s="1">
+        <v>12.56</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="E73" s="6" t="e">
+        <f>B73+#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B74" s="1">
         <v>0.12035999999999999</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E74" s="6">
         <f t="shared" si="1"/>
         <v>0.12035999999999999</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F74" s="1">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C75" s="1">
         <v>9.1739999999999995</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D75" s="1">
         <v>6.76</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B76" s="1">
         <v>0.14280000000000001</v>
       </c>
-      <c r="E60" s="6">
-        <f t="shared" ref="E60:E91" si="2">B60+D60</f>
+      <c r="E76" s="6">
+        <f t="shared" ref="E76:E107" si="2">B76+D76</f>
         <v>0.14280000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B77" s="1">
         <v>0.12628</v>
       </c>
-      <c r="E61" s="6">
+      <c r="C77" s="1">
+        <v>4.3490000000000002</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2.9710000000000001</v>
+      </c>
+      <c r="E77" s="6">
         <f t="shared" si="2"/>
-        <v>0.12628</v>
-      </c>
-      <c r="F61" s="1">
+        <v>3.09728</v>
+      </c>
+      <c r="F77" s="1">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B78" s="1">
         <v>0.19905</v>
       </c>
-      <c r="E62" s="6">
-        <f t="shared" si="2"/>
-        <v>0.19905</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="C78" s="1">
+        <v>6.6539999999999999</v>
+      </c>
+      <c r="D78" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="E78" s="6">
+        <f>B78+D78</f>
+        <v>3.6390500000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B79" s="1">
         <v>9.0279999999999999E-2</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E79" s="6">
         <f t="shared" si="2"/>
         <v>9.0279999999999999E-2</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F79" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B80" s="1">
         <v>0.25972000000000001</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C80" s="1">
         <v>14.5</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D80" s="1">
         <v>4.2519</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E80" s="6">
         <f t="shared" si="2"/>
         <v>4.5116199999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B81" s="1">
         <v>0.16172</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E81" s="6">
         <f t="shared" si="2"/>
         <v>0.16172</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F81" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B82" s="1">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E82" s="6">
         <f t="shared" si="2"/>
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B83" s="1">
         <v>0.29918</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E83" s="6">
         <f t="shared" si="2"/>
         <v>0.29918</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F83" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B84" s="1">
         <v>0.11191</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E84" s="6">
         <f t="shared" si="2"/>
         <v>0.11191</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B85" s="1">
         <v>0.20174</v>
       </c>
-      <c r="E69" s="6">
-        <f>B69+D35</f>
+      <c r="E85" s="6">
+        <f>B85+D51</f>
         <v>4.8607399999999998</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F85" s="1">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B86" s="1">
         <v>0.12363</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E86" s="6">
         <f t="shared" si="2"/>
         <v>0.12363</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B87" s="1">
         <v>0.1925</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E87" s="6">
         <f t="shared" si="2"/>
         <v>0.1925</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F87" s="1">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B88" s="1">
         <v>8.3280000000000007E-2</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E88" s="6">
         <f t="shared" si="2"/>
         <v>8.3280000000000007E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B89" s="1">
         <v>0.23799999999999999</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E89" s="6">
         <f t="shared" si="2"/>
         <v>0.23799999999999999</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F89" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B90" s="1">
         <v>0.12200999999999999</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E90" s="6">
         <f t="shared" si="2"/>
         <v>0.12200999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B91" s="1">
         <v>0.15851999999999999</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E91" s="6">
         <f t="shared" si="2"/>
         <v>0.15851999999999999</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F91" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B92" s="1">
         <v>0.12623000000000001</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E92" s="6">
         <f t="shared" si="2"/>
         <v>0.12623000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B93" s="1">
         <v>0.19725000000000001</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E93" s="6">
         <f t="shared" si="2"/>
         <v>0.19725000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B94" s="1">
         <v>0.13694000000000001</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E94" s="6">
         <f t="shared" si="2"/>
         <v>0.13694000000000001</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F94" s="1">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B95" s="1">
         <v>0.11362</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E95" s="6">
         <f t="shared" si="2"/>
         <v>0.11362</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B96" s="1">
         <v>0.44784000000000002</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E96" s="6">
         <f t="shared" si="2"/>
         <v>0.44784000000000002</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F96" s="1">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B97" s="1">
         <v>0.27638000000000001</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E97" s="6">
         <f t="shared" si="2"/>
         <v>0.27638000000000001</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F97" s="1">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B98" s="1">
         <v>9.8710000000000006E-2</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E98" s="6">
         <f t="shared" si="2"/>
         <v>9.8710000000000006E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B99" s="1">
         <v>0.21001</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E99" s="6">
         <f t="shared" si="2"/>
         <v>0.21001</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F99" s="1">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B100" s="1">
         <v>0.19574</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E100" s="6">
         <f t="shared" si="2"/>
         <v>0.19574</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B101" s="1">
         <v>6.2740000000000004E-2</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E101" s="6">
         <f t="shared" si="2"/>
         <v>6.2740000000000004E-2</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F101" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B102" s="1">
         <v>0.16908000000000001</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E102" s="6">
         <f t="shared" si="2"/>
         <v>0.16908000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B103" s="1">
         <v>0.15723999999999999</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E103" s="6">
         <f t="shared" si="2"/>
         <v>0.15723999999999999</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F103" s="1">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B104" s="1">
         <v>5.7930000000000002E-2</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E104" s="6">
         <f t="shared" si="2"/>
         <v>5.7930000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B105" s="1">
         <v>0.20799999999999999</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E105" s="6">
         <f t="shared" si="2"/>
         <v>0.20799999999999999</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F105" s="1">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B106" s="1">
         <v>0.14298</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E106" s="6">
         <f t="shared" si="2"/>
         <v>0.14298</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B107" s="1">
         <v>0.14215</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E107" s="6">
         <f t="shared" si="2"/>
         <v>0.14215</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F107" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B108" s="1">
         <v>9.5149999999999998E-2</v>
       </c>
-      <c r="E92" s="6">
-        <f t="shared" ref="E92:E123" si="3">B92+D92</f>
+      <c r="E108" s="6">
+        <f t="shared" ref="E108:E139" si="3">B108+D108</f>
         <v>9.5149999999999998E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B109" s="1">
         <v>0.19455</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E109" s="6">
         <f t="shared" si="3"/>
         <v>0.19455</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F109" s="1">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B110" s="1">
         <v>0.1221</v>
       </c>
-      <c r="E94" s="6">
+      <c r="E110" s="6">
         <f t="shared" si="3"/>
         <v>0.1221</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B111" s="1">
         <v>9.3380000000000005E-2</v>
       </c>
-      <c r="E95" s="6">
+      <c r="E111" s="6">
         <f t="shared" si="3"/>
         <v>9.3380000000000005E-2</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F111" s="1">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B112" s="1">
         <v>0.10866000000000001</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E112" s="6">
         <f t="shared" si="3"/>
         <v>0.10866000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B113" s="1">
         <v>0.21836</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E113" s="6">
         <f t="shared" si="3"/>
         <v>0.21836</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F113" s="1">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B114" s="1">
         <v>0.11178</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E114" s="6">
         <f t="shared" si="3"/>
         <v>0.11178</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B115" s="1">
         <v>0.24346999999999999</v>
       </c>
-      <c r="E99" s="6">
+      <c r="E115" s="6">
         <f t="shared" si="3"/>
         <v>0.24346999999999999</v>
       </c>
-      <c r="F99" s="1">
+      <c r="F115" s="1">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B116" s="1">
         <v>8.0930000000000002E-2</v>
       </c>
-      <c r="E100" s="6">
+      <c r="E116" s="6">
         <f t="shared" si="3"/>
         <v>8.0930000000000002E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E101" s="6">
+      <c r="C117" s="1">
+        <v>24.3</v>
+      </c>
+      <c r="D117" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="E117" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B118" s="1">
         <v>0.15595999999999999</v>
       </c>
-      <c r="E102" s="6">
+      <c r="E118" s="6">
         <f t="shared" si="3"/>
         <v>0.15595999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="E103" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B104" s="1">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="E104" s="6">
-        <f t="shared" si="3"/>
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C105" s="1">
-        <f>12.688+11.96</f>
-        <v>24.648000000000003</v>
-      </c>
-      <c r="D105" s="1">
-        <v>9.609</v>
-      </c>
-      <c r="E105" s="6">
-        <f t="shared" si="3"/>
-        <v>9.609</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B106" s="1">
-        <v>0.1057</v>
-      </c>
-      <c r="E106" s="6">
-        <f t="shared" si="3"/>
-        <v>0.1057</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E107" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B108" s="1">
-        <v>8.4400000000000003E-2</v>
-      </c>
-      <c r="E108" s="6">
-        <f t="shared" si="3"/>
-        <v>8.4400000000000003E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B109" s="1">
-        <v>0.11948</v>
-      </c>
-      <c r="E109" s="6">
-        <f t="shared" si="3"/>
-        <v>0.11948</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E110" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B111" s="1">
-        <v>0.13216</v>
-      </c>
-      <c r="E111" s="6">
-        <f t="shared" si="3"/>
-        <v>0.13216</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E112" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E113" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B114" s="1">
-        <v>0.1056</v>
-      </c>
-      <c r="E114" s="6">
-        <f t="shared" si="3"/>
-        <v>0.1056</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E115" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B116" s="1">
-        <f>0.05+0.021</f>
-        <v>7.1000000000000008E-2</v>
-      </c>
-      <c r="E116" s="6">
-        <f t="shared" si="3"/>
-        <v>7.1000000000000008E-2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E117" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B118" s="1">
-        <v>5.5550000000000002E-2</v>
-      </c>
-      <c r="E118" s="6">
-        <f t="shared" si="3"/>
-        <v>5.5550000000000002E-2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="E119" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B120" s="1">
-        <v>9.0660000000000004E-2</v>
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="C120" s="1">
+        <v>29.88</v>
+      </c>
+      <c r="D120" s="1">
+        <v>8.3000000000000007</v>
       </c>
       <c r="E120" s="6">
         <f t="shared" si="3"/>
-        <v>9.0660000000000004E-2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9.2280000000000015</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
-        <v>185</v>
+        <v>193</v>
+      </c>
+      <c r="C121" s="1">
+        <f>12.688+11.96</f>
+        <v>24.648000000000003</v>
+      </c>
+      <c r="D121" s="1">
+        <v>9.609</v>
       </c>
       <c r="E121" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9.609</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B122" s="1">
-        <v>0.21970000000000001</v>
+        <v>0.1057</v>
+      </c>
+      <c r="C122" s="1">
+        <v>18.41</v>
+      </c>
+      <c r="D122" s="1">
+        <v>7.55</v>
       </c>
       <c r="E122" s="6">
         <f t="shared" si="3"/>
-        <v>0.21970000000000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7.6556999999999995</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E123" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B124" s="1">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="C124" s="1">
+        <v>15.15</v>
+      </c>
+      <c r="D124" s="1">
+        <v>11.77</v>
+      </c>
+      <c r="E124" s="6">
+        <f t="shared" si="3"/>
+        <v>11.8544</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0.11948</v>
+      </c>
+      <c r="C125" s="1">
+        <v>24.44</v>
+      </c>
+      <c r="D125" s="1">
+        <v>8.02</v>
+      </c>
+      <c r="E125" s="6">
+        <f t="shared" si="3"/>
+        <v>8.1394799999999989</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E126" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0.13216</v>
+      </c>
+      <c r="E127" s="6">
+        <f t="shared" si="3"/>
+        <v>0.13216</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E128" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C129" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="D129" s="1">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E129" s="6">
+        <f t="shared" si="3"/>
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0.1056</v>
+      </c>
+      <c r="C130" s="1">
+        <v>23.53</v>
+      </c>
+      <c r="D130" s="1">
+        <v>7.34</v>
+      </c>
+      <c r="E130" s="6">
+        <f t="shared" si="3"/>
+        <v>7.4455999999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E131" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132" s="1">
+        <f>0.05+0.021</f>
+        <v>7.1000000000000008E-2</v>
+      </c>
+      <c r="E132" s="6">
+        <f t="shared" si="3"/>
+        <v>7.1000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C133" s="1">
+        <v>21.69</v>
+      </c>
+      <c r="D133" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="E133" s="6">
+        <f t="shared" si="3"/>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" s="1">
+        <v>5.5550000000000002E-2</v>
+      </c>
+      <c r="C134" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="D134" s="1">
+        <v>9.4719999999999995</v>
+      </c>
+      <c r="E134" s="6">
+        <f t="shared" si="3"/>
+        <v>9.5275499999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E135" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B136" s="1">
+        <v>9.0660000000000004E-2</v>
+      </c>
+      <c r="E136" s="6">
+        <f t="shared" si="3"/>
+        <v>9.0660000000000004E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E137" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B138" s="1">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="E138" s="6">
+        <f t="shared" si="3"/>
+        <v>0.21970000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E139" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B140" s="1">
         <v>9.826E-2</v>
       </c>
-      <c r="E124" s="6">
-        <f t="shared" ref="E124:E155" si="4">B124+D124</f>
-        <v>9.826E-2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
+      <c r="C140" s="1">
+        <v>17</v>
+      </c>
+      <c r="D140" s="1">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="E140" s="6">
+        <f t="shared" ref="E140:E187" si="4">B140+D140</f>
+        <v>4.2082600000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E125" s="6">
+      <c r="C141" s="1">
+        <v>24.13</v>
+      </c>
+      <c r="D141" s="1">
+        <v>15.47</v>
+      </c>
+      <c r="E141" s="6">
+        <f t="shared" si="4"/>
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B142" s="1">
+        <v>6.2850000000000003E-2</v>
+      </c>
+      <c r="E142" s="6">
+        <f t="shared" si="4"/>
+        <v>6.2850000000000003E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C143" s="1">
+        <v>26.07</v>
+      </c>
+      <c r="D143" s="1">
+        <v>12.37</v>
+      </c>
+      <c r="E143" s="6">
+        <f t="shared" si="4"/>
+        <v>12.37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0.10732</v>
+      </c>
+      <c r="C144" s="1">
+        <v>24.73</v>
+      </c>
+      <c r="D144" s="1">
+        <v>14.55</v>
+      </c>
+      <c r="E144" s="6">
+        <f t="shared" si="4"/>
+        <v>14.65732</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C145" s="1">
+        <v>23.54</v>
+      </c>
+      <c r="D145" s="1">
+        <f>17.51+6.95</f>
+        <v>24.46</v>
+      </c>
+      <c r="E145" s="6">
+        <f t="shared" si="4"/>
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="1">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="E146" s="6">
+        <f t="shared" si="4"/>
+        <v>8.5599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C147" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="D147" s="1">
+        <v>6.64</v>
+      </c>
+      <c r="E147" s="6">
+        <f t="shared" si="4"/>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C149" s="1">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="D149" s="1">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C153" s="1">
+        <v>22.48</v>
+      </c>
+      <c r="D153" s="1">
+        <v>10.37</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C154" s="1">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="D154" s="1">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C158" s="1">
+        <v>40.869999999999997</v>
+      </c>
+      <c r="D158" s="1">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C160" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="D160" s="1">
+        <v>8.7889999999999997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C161" s="1">
+        <v>25.98</v>
+      </c>
+      <c r="D161" s="1">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C163" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="D163" s="1">
+        <v>13.58</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B164" s="1">
+        <v>9.7339999999999996E-2</v>
+      </c>
+      <c r="E164" s="6">
+        <f t="shared" si="4"/>
+        <v>9.7339999999999996E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B165" s="1">
+        <v>0.11348</v>
+      </c>
+      <c r="E165" s="6">
+        <f t="shared" si="4"/>
+        <v>0.11348</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B166" s="1">
+        <v>7.4529999999999999E-2</v>
+      </c>
+      <c r="E166" s="6">
+        <f t="shared" si="4"/>
+        <v>7.4529999999999999E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B167" s="1">
+        <v>0.11441</v>
+      </c>
+      <c r="E167" s="6">
+        <f t="shared" si="4"/>
+        <v>0.11441</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B168" s="1">
+        <v>0.11364</v>
+      </c>
+      <c r="E168" s="6">
+        <f t="shared" si="4"/>
+        <v>0.11364</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B169" s="1">
+        <v>0.10153</v>
+      </c>
+      <c r="E169" s="6">
+        <f t="shared" si="4"/>
+        <v>0.10153</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B170" s="1">
+        <v>9.1689999999999994E-2</v>
+      </c>
+      <c r="E170" s="6">
+        <f t="shared" si="4"/>
+        <v>9.1689999999999994E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B171" s="1">
+        <v>0.1221</v>
+      </c>
+      <c r="E171" s="6">
+        <f t="shared" si="4"/>
+        <v>0.1221</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B172" s="1">
+        <v>0.14896999999999999</v>
+      </c>
+      <c r="E172" s="6">
+        <f t="shared" si="4"/>
+        <v>0.14896999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B173" s="1">
+        <v>8.6440000000000003E-2</v>
+      </c>
+      <c r="E173" s="6">
+        <f t="shared" si="4"/>
+        <v>8.6440000000000003E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B174" s="1">
+        <v>0.14696000000000001</v>
+      </c>
+      <c r="E174" s="6">
+        <f t="shared" si="4"/>
+        <v>0.14696000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B175" s="1">
+        <v>0.11192000000000001</v>
+      </c>
+      <c r="E175" s="6">
+        <f t="shared" si="4"/>
+        <v>0.11192000000000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B176" s="1">
+        <v>0.11283</v>
+      </c>
+      <c r="E176" s="6">
+        <f t="shared" si="4"/>
+        <v>0.11283</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B177" s="1">
+        <v>0.114523</v>
+      </c>
+      <c r="E177" s="6">
+        <f t="shared" si="4"/>
+        <v>0.114523</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B178" s="1">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E178" s="6">
+        <f t="shared" si="4"/>
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B179" s="1">
+        <v>0.10724</v>
+      </c>
+      <c r="E179" s="6">
+        <f t="shared" si="4"/>
+        <v>0.10724</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B180" s="1">
+        <v>8.9440000000000006E-2</v>
+      </c>
+      <c r="E180" s="6">
+        <f t="shared" si="4"/>
+        <v>8.9440000000000006E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C181" s="1">
+        <v>10.477</v>
+      </c>
+      <c r="D181" s="1">
+        <v>6.5220000000000002</v>
+      </c>
+      <c r="E181" s="6">
+        <f t="shared" si="4"/>
+        <v>6.5220000000000002</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B182" s="1">
+        <v>4.2770000000000002E-2</v>
+      </c>
+      <c r="E182" s="6">
+        <f t="shared" si="4"/>
+        <v>4.2770000000000002E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E183" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B126" s="1">
-        <v>6.2850000000000003E-2</v>
-      </c>
-      <c r="E126" s="6">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B184" s="3">
+        <v>0</v>
+      </c>
+      <c r="C184" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="D184" s="1">
+        <v>4.0970000000000004</v>
+      </c>
+      <c r="E184" s="6">
         <f t="shared" si="4"/>
-        <v>6.2850000000000003E-2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E127" s="6">
+        <v>4.0970000000000004</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E185" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B128" s="1">
-        <v>0.10732</v>
-      </c>
-      <c r="E128" s="6">
-        <f t="shared" si="4"/>
-        <v>0.10732</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E129" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B130" s="1">
-        <v>8.5599999999999996E-2</v>
-      </c>
-      <c r="E130" s="6">
-        <f t="shared" si="4"/>
-        <v>8.5599999999999996E-2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E131" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B132" s="1">
-        <v>9.7339999999999996E-2</v>
-      </c>
-      <c r="E132" s="6">
-        <f t="shared" si="4"/>
-        <v>9.7339999999999996E-2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B133" s="1">
-        <v>0.11348</v>
-      </c>
-      <c r="E133" s="6">
-        <f t="shared" si="4"/>
-        <v>0.11348</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B134" s="1">
-        <v>7.4529999999999999E-2</v>
-      </c>
-      <c r="E134" s="6">
-        <f t="shared" si="4"/>
-        <v>7.4529999999999999E-2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B135" s="1">
-        <v>0.11441</v>
-      </c>
-      <c r="E135" s="6">
-        <f t="shared" si="4"/>
-        <v>0.11441</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B136" s="1">
-        <v>0.11364</v>
-      </c>
-      <c r="E136" s="6">
-        <f t="shared" si="4"/>
-        <v>0.11364</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B137" s="1">
-        <v>0.10153</v>
-      </c>
-      <c r="E137" s="6">
-        <f t="shared" si="4"/>
-        <v>0.10153</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B138" s="1">
-        <v>9.1689999999999994E-2</v>
-      </c>
-      <c r="E138" s="6">
-        <f t="shared" si="4"/>
-        <v>9.1689999999999994E-2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B139" s="1">
-        <v>0.1221</v>
-      </c>
-      <c r="E139" s="6">
-        <f t="shared" si="4"/>
-        <v>0.1221</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B140" s="1">
-        <v>0.14896999999999999</v>
-      </c>
-      <c r="E140" s="6">
-        <f t="shared" si="4"/>
-        <v>0.14896999999999999</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B141" s="1">
-        <v>8.6440000000000003E-2</v>
-      </c>
-      <c r="E141" s="6">
-        <f t="shared" si="4"/>
-        <v>8.6440000000000003E-2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B142" s="1">
-        <v>0.14696000000000001</v>
-      </c>
-      <c r="E142" s="6">
-        <f t="shared" si="4"/>
-        <v>0.14696000000000001</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B143" s="1">
-        <v>0.11192000000000001</v>
-      </c>
-      <c r="E143" s="6">
-        <f t="shared" si="4"/>
-        <v>0.11192000000000001</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B144" s="1">
-        <v>0.11283</v>
-      </c>
-      <c r="E144" s="6">
-        <f t="shared" si="4"/>
-        <v>0.11283</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B145" s="1">
-        <v>0.114523</v>
-      </c>
-      <c r="E145" s="6">
-        <f t="shared" si="4"/>
-        <v>0.114523</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B146" s="1">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="E146" s="6">
-        <f t="shared" si="4"/>
-        <v>0.10299999999999999</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B147" s="1">
-        <v>0.10724</v>
-      </c>
-      <c r="E147" s="6">
-        <f t="shared" si="4"/>
-        <v>0.10724</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B148" s="1">
-        <v>8.9440000000000006E-2</v>
-      </c>
-      <c r="E148" s="6">
-        <f t="shared" si="4"/>
-        <v>8.9440000000000006E-2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E149" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B150" s="1">
-        <v>4.2770000000000002E-2</v>
-      </c>
-      <c r="E150" s="6">
-        <f t="shared" si="4"/>
-        <v>4.2770000000000002E-2</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E151" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E152" s="6" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E153" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="3" t="s">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B186" s="1">
         <v>6.2140000000000001E-2</v>
       </c>
-      <c r="E154" s="6">
+      <c r="E186" s="6">
         <f t="shared" si="4"/>
         <v>6.2140000000000001E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E155" s="6">
+      <c r="C187" s="1">
+        <v>3.47</v>
+      </c>
+      <c r="D187" s="1">
+        <v>3.306</v>
+      </c>
+      <c r="E187" s="6">
         <f t="shared" si="4"/>
+        <v>3.306</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B188" s="1">
+        <v>3.8440000000000002E-2</v>
+      </c>
+      <c r="C188" s="1">
+        <v>5.375</v>
+      </c>
+      <c r="D188" s="1">
+        <v>1.831</v>
+      </c>
+      <c r="E188" s="6">
+        <f t="shared" ref="E188:E189" si="5">B188+D188</f>
+        <v>1.86944</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B189" s="1">
+        <v>6.8339999999999998E-2</v>
+      </c>
+      <c r="C189" s="1">
+        <v>8.2449999999999992</v>
+      </c>
+      <c r="D189" s="1">
+        <v>3.0609999999999999</v>
+      </c>
+      <c r="E189" s="6">
+        <f t="shared" si="5"/>
+        <v>3.12934</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C190" s="1">
+        <v>5.4260000000000002</v>
+      </c>
+      <c r="D190" s="1">
+        <v>3.8471500000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E191" s="6">
+        <f>B191+D191</f>
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B156" s="1">
-        <v>3.8440000000000002E-2</v>
-      </c>
-      <c r="E156" s="6">
-        <f t="shared" ref="E156:E187" si="5">B156+D156</f>
-        <v>3.8440000000000002E-2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B157" s="1">
-        <v>6.8339999999999998E-2</v>
-      </c>
-      <c r="E157" s="6">
-        <f t="shared" si="5"/>
-        <v>6.8339999999999998E-2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C158" s="1">
-        <v>5.4260000000000002</v>
-      </c>
-      <c r="D158" s="1">
-        <v>3.8471500000000001</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E159" s="6">
-        <f>B159+D159</f>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B192" s="1">
+        <v>6.3759999999999997E-2</v>
+      </c>
+      <c r="C192" s="1">
+        <v>17.46</v>
+      </c>
+      <c r="D192" s="1">
+        <v>9.7089999999999996</v>
+      </c>
+      <c r="E192" s="6">
+        <f>B192+D192</f>
+        <v>9.7727599999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E193" s="6">
+        <f>B193+D193</f>
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B160" s="1">
-        <v>6.3759999999999997E-2</v>
-      </c>
-      <c r="E160" s="6">
-        <f>B160+D160</f>
-        <v>6.3759999999999997E-2</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E161" s="6">
-        <f>B161+D161</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="7" t="s">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C194" s="1">
         <v>11.588010000000001</v>
       </c>
-      <c r="D162" s="1">
+      <c r="D194" s="1">
         <v>7.3784799999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="3" t="s">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B195" s="1">
         <v>6.6970000000000002E-2</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C195" s="1">
         <v>15.71</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D195" s="1">
         <v>6.0713499999999998</v>
       </c>
-      <c r="E163" s="6">
-        <f t="shared" ref="E163:E197" si="6">B163+D163</f>
+      <c r="E195" s="6">
+        <f t="shared" ref="E195:E245" si="6">B195+D195</f>
         <v>6.1383200000000002</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C164" s="1">
+      <c r="C196" s="1">
         <v>10.210000000000001</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D196" s="1">
         <v>8.2289999999999992</v>
       </c>
-      <c r="E164" s="6">
+      <c r="E196" s="6">
         <f t="shared" si="6"/>
         <v>8.2289999999999992</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E165" s="6">
+      <c r="E197" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="3" t="s">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B198" s="1">
         <v>5.3719999999999997E-2</v>
       </c>
-      <c r="E166" s="6">
+      <c r="E198" s="6">
         <f t="shared" si="6"/>
         <v>5.3719999999999997E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C167" s="1">
+      <c r="C199" s="1">
         <v>7.5597799999999999</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D199" s="1">
         <v>4.2313200000000002</v>
       </c>
-      <c r="E167" s="6">
+      <c r="E199" s="6">
         <f t="shared" si="6"/>
         <v>4.2313200000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="3" t="s">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B200" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E168" s="6" t="e">
+      <c r="E200" s="6" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E169" s="6">
+      <c r="E201" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="3" t="s">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B170" s="1">
+      <c r="B202" s="1">
         <v>4.9099999999999998E-2</v>
       </c>
-      <c r="E170" s="6">
+      <c r="E202" s="6">
         <f t="shared" si="6"/>
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E171" s="6">
+      <c r="E203" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="3" t="s">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B172" s="1">
+      <c r="B204" s="1">
         <v>4.1309999999999999E-2</v>
       </c>
-      <c r="E172" s="6">
+      <c r="E204" s="6">
         <f t="shared" si="6"/>
         <v>4.1309999999999999E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E173" s="6">
+      <c r="E205" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A174" s="3" t="s">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B174" s="1">
+      <c r="B206" s="1">
         <v>2.5819999999999999E-2</v>
       </c>
-      <c r="E174" s="6">
+      <c r="C206" s="1">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="D206" s="1">
+        <v>4.1459999999999999</v>
+      </c>
+      <c r="E206" s="6">
         <f t="shared" si="6"/>
-        <v>2.5819999999999999E-2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
+        <v>4.1718200000000003</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E175" s="6">
+      <c r="E207" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="3" t="s">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B176" s="1">
+      <c r="B208" s="1">
         <v>7.7539999999999998E-2</v>
       </c>
-      <c r="C176" s="1">
+      <c r="C208" s="1">
         <v>9.82</v>
       </c>
-      <c r="D176" s="1">
+      <c r="D208" s="1">
         <v>5.9350699999999996</v>
       </c>
-      <c r="E176" s="6">
+      <c r="E208" s="6">
         <f t="shared" si="6"/>
         <v>6.0126099999999996</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E177" s="6">
+      <c r="E209" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="3" t="s">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B178" s="1">
+      <c r="B210" s="1">
         <v>2.2429999999999999E-2</v>
       </c>
-      <c r="E178" s="6">
+      <c r="E210" s="6">
         <f t="shared" si="6"/>
         <v>2.2429999999999999E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E179" s="6">
+      <c r="C211" s="1">
+        <v>8.92</v>
+      </c>
+      <c r="D211" s="1">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E211" s="6">
+        <f t="shared" si="6"/>
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B212" s="1">
+        <v>4.1459999999999997E-2</v>
+      </c>
+      <c r="E212" s="6">
+        <f t="shared" si="6"/>
+        <v>4.1459999999999997E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E213" s="6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B180" s="1">
-        <v>4.1459999999999997E-2</v>
-      </c>
-      <c r="E180" s="6">
-        <f t="shared" si="6"/>
-        <v>4.1459999999999997E-2</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E181" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" s="2" t="s">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C219" s="1">
+        <v>2.65</v>
+      </c>
+      <c r="D219" s="1">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B182" s="1">
+      <c r="B230" s="1">
         <v>0.4834</v>
       </c>
-      <c r="E182" s="6">
+      <c r="E230" s="6">
         <f t="shared" si="6"/>
         <v>0.4834</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" s="2" t="s">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B183" s="1">
+      <c r="B231" s="1">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="C183" s="2"/>
-      <c r="E183" s="6">
+      <c r="C231" s="2"/>
+      <c r="E231" s="6">
         <f t="shared" si="6"/>
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" s="2" t="s">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B184" s="1">
+      <c r="B232" s="1">
         <v>9.5170000000000005E-2</v>
       </c>
-      <c r="E184" s="6">
+      <c r="E232" s="6">
         <f t="shared" si="6"/>
         <v>9.5170000000000005E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A185" s="2" t="s">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B185" s="1">
+      <c r="B233" s="1">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="E185" s="6">
+      <c r="E233" s="6">
         <f t="shared" si="6"/>
         <v>7.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A186" s="2" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B186" s="1">
+      <c r="B234" s="1">
         <v>0.17377999999999999</v>
       </c>
-      <c r="E186" s="6">
+      <c r="E234" s="6">
         <f t="shared" si="6"/>
         <v>0.17377999999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A187" s="2" t="s">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B187" s="1">
+      <c r="B235" s="1">
         <v>4.02E-2</v>
       </c>
-      <c r="C187" s="2"/>
-      <c r="E187" s="6">
+      <c r="C235" s="2"/>
+      <c r="E235" s="6">
         <f t="shared" si="6"/>
         <v>4.02E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" s="2" t="s">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B188" s="1">
+      <c r="B236" s="1">
         <v>6.0100000000000001E-2</v>
       </c>
-      <c r="E188" s="6">
+      <c r="E236" s="6">
         <f t="shared" si="6"/>
         <v>6.0100000000000001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A189" s="2" t="s">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B189" s="1">
+      <c r="B237" s="1">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="C189" s="2"/>
-      <c r="E189" s="6">
+      <c r="C237" s="2"/>
+      <c r="E237" s="6">
         <f t="shared" si="6"/>
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B190" s="1">
+      <c r="B238" s="1">
         <v>8.9099999999999999E-2</v>
       </c>
-      <c r="E190" s="6">
+      <c r="E238" s="6">
         <f t="shared" si="6"/>
         <v>8.9099999999999999E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B191" s="1">
+      <c r="B239" s="1">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="E191" s="6">
+      <c r="E239" s="6">
         <f t="shared" si="6"/>
         <v>8.4099999999999994E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A192" s="2" t="s">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B192" s="1">
+      <c r="B240" s="1">
         <v>6.9699999999999998E-2</v>
       </c>
-      <c r="E192" s="6">
+      <c r="E240" s="6">
         <f t="shared" si="6"/>
         <v>6.9699999999999998E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="2" t="s">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B193" s="1">
+      <c r="B241" s="1">
         <v>3.7199999999999997E-2</v>
       </c>
-      <c r="C193" s="2"/>
-      <c r="E193" s="6">
+      <c r="C241" s="2"/>
+      <c r="E241" s="6">
         <f t="shared" si="6"/>
         <v>3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" s="2" t="s">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B194" s="1">
+      <c r="B242" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C194" s="2"/>
-      <c r="E194" s="6">
+      <c r="C242" s="2"/>
+      <c r="E242" s="6">
         <f t="shared" si="6"/>
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B195" s="1">
+      <c r="B243" s="1">
         <v>0.47</v>
       </c>
-      <c r="C195" s="2"/>
-      <c r="E195" s="6">
+      <c r="C243" s="2"/>
+      <c r="E243" s="6">
         <f t="shared" si="6"/>
         <v>0.47</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B244" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E196" s="6" t="e">
+      <c r="E244" s="6" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A197" s="2" t="s">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B197" s="1">
+      <c r="B245" s="1">
         <v>0.44400000000000001</v>
       </c>
-      <c r="C197" s="2"/>
-      <c r="E197" s="6">
+      <c r="C245" s="2"/>
+      <c r="E245" s="6">
         <f t="shared" si="6"/>
         <v>0.44400000000000001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F193">
-      <sortCondition ref="A1:A193"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F241">
+      <sortCondition ref="A1:A241"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>